<commit_message>
Improved xlsx file and fixed bug with overlapping days
</commit_message>
<xml_diff>
--- a/test_dia.xlsx
+++ b/test_dia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Belen/Dropbox/Programacion/Proyectos/Iberdrolux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA7A2D3-9C37-E641-813D-497E59F6A5BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C0B37C-C974-3749-8A46-A8627609EC72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{282E9E91-F784-6B4B-BA20-4F197C46D5EC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Hora</t>
   </si>
@@ -68,13 +68,22 @@
     <t>Precio por kW/año de potencia (€):</t>
   </si>
   <si>
-    <t>Inicio hora bonificada:</t>
-  </si>
-  <si>
-    <t>Fin hora bonificada:</t>
-  </si>
-  <si>
     <t>COSTE TOTAL (€):</t>
+  </si>
+  <si>
+    <t>Marque X si la hora está bonificada:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>*** INSTRUCCIONES ***</t>
+  </si>
+  <si>
+    <t>Modifique las celdas con doble borde para introducir sus datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSUMO TOTAL (kW): </t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -106,13 +115,264 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,583 +687,800 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697522F4-44C9-8C4D-B60F-C35EB184269D}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="167" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="7" max="7" width="3.1640625" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E1" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10">
+        <v>42736</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="6">
         <v>365</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
+        <v>0.17116600000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9">
+        <f>SUM(E6:E29)</f>
+        <v>18.86972923749315</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6">
         <v>8.5875000000000007E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>42736</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>0.17116600000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <f>SUM(E6:E30)</f>
-        <v>18.448903443493148</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <f>SUM(C6:C29)</f>
+        <v>13.261000000000001</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>57.23</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3">
-        <v>23</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>602</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <f>B6/1000</f>
         <v>0.60199999999999998</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f>E6-($F$2*$F$3/$F$1)</f>
         <v>5.1696749999999958E-2</v>
       </c>
-      <c r="E6">
-        <f>IF(ISBLANK($I$3),  $F$2*$F$3/$F$1 + $I$1*$C6,  IF(AND($A6&gt;=$I$3,  $A6&lt;=$I$4),  $F$2*$F$3/$F$1 + $I$2*$C6,  $F$2*$F$3/$F$1 + $I$1*$C6))</f>
+      <c r="E6" s="2">
+        <f>IF(I6="X", C6*$I$2,C6*$I$1)+($F$2*$F$3/$F$1)</f>
         <v>0.77295154452054782</v>
       </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>548</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <f t="shared" ref="C7:C30" si="0">B7/1000</f>
         <v>0.54800000000000004</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" ref="D7:D29" si="1">E7-($F$2*$F$3/$F$1)</f>
         <v>4.7059500000000032E-2</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E30" si="2">IF(ISBLANK($I$3),  $F$2*$F$3/$F$1 + $I$1*$C7,  IF(AND($A7&gt;=$I$3,  $A7&lt;=$I$4),  $F$2*$F$3/$F$1 + $I$2*$C7,  $F$2*$F$3/$F$1 + $I$1*$C7))</f>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:E29" si="2">IF(I7="X", C7*$I$2,C7*$I$1)+($F$2*$F$3/$F$1)</f>
         <v>0.76831429452054789</v>
       </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>942</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>0.94199999999999995</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
         <v>8.0894250000000056E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>0.80214904452054792</v>
       </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="7">
         <v>649</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>0.64900000000000002</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f t="shared" si="1"/>
         <v>5.5732875000000015E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
         <v>0.77698766952054787</v>
       </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <v>233</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>0.23300000000000001</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f t="shared" si="1"/>
         <v>2.0008875000000037E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="2"/>
         <v>0.7412636695205479</v>
       </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="7">
         <v>102</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>0.10199999999999999</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f t="shared" si="1"/>
         <v>8.7592499999999962E-3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="2"/>
         <v>0.73001404452054786</v>
       </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>124</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>0.124</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <f t="shared" si="1"/>
         <v>1.064849999999995E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="2"/>
         <v>0.73190329452054781</v>
       </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="3">
+        <v>6</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="7">
         <v>85</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <f t="shared" si="1"/>
         <v>7.2993749999999968E-3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="2"/>
         <v>0.72855416952054786</v>
       </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="3">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>155</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>0.155</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <f t="shared" si="1"/>
         <v>1.331062500000002E-2</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
         <v>0.73456541952054788</v>
       </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="3">
+        <v>8</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>9</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <v>287</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>0.28699999999999998</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <f t="shared" si="1"/>
         <v>2.4646124999999963E-2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <f t="shared" si="2"/>
         <v>0.74590091952054782</v>
       </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="3">
+        <v>9</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="7">
         <v>244</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>0.24399999999999999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <f t="shared" si="1"/>
         <v>2.0953499999999958E-2</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <f t="shared" si="2"/>
         <v>0.74220829452054782</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="3">
+        <v>10</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>11</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="7">
         <v>283</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>0.28299999999999997</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <f t="shared" si="1"/>
         <v>2.4302625000000022E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
         <v>0.74555741952054788</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="3">
+        <v>11</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>12</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="7">
         <v>654</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>0.65400000000000003</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <f t="shared" si="1"/>
         <v>5.6162249999999969E-2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <f t="shared" si="2"/>
         <v>0.77741704452054783</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="3">
+        <v>12</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7">
         <v>486</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>0.48599999999999999</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <f t="shared" si="1"/>
         <v>4.1735250000000002E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
         <v>0.76299004452054786</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="3">
+        <v>13</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>14</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>775</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>6.6553124999999991E-2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
-        <v>0.78780791952054785</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13265364999999996</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.85390844452054782</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="3">
+        <v>14</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>15</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="7">
         <v>699</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>0.69899999999999995</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>6.0026625E-2</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>0.78128141952054786</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11964503400000004</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8408998285205479</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="3">
+        <v>15</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>16</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>377</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <f t="shared" si="0"/>
         <v>0.377</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>3.2374875000000025E-2</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>0.75362966952054788</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>6.452958200000003E-2</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="2"/>
+        <v>0.78578437652054789</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="3">
+        <v>16</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>17</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>314</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <f t="shared" si="0"/>
         <v>0.314</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>2.6964749999999982E-2</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="2"/>
-        <v>0.74821954452054784</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>5.3746124000000006E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="2"/>
+        <v>0.77500091852054787</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="3">
+        <v>17</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>18</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <v>592</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>0.59199999999999997</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
-        <v>5.083800000000005E-2</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="2"/>
-        <v>0.77209279452054791</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="D24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.101330272</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="2"/>
+        <v>0.82258506652054786</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="3">
+        <v>18</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>19</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="7">
         <v>657</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <f t="shared" si="0"/>
         <v>0.65700000000000003</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>5.6419875000000008E-2</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="2"/>
-        <v>0.77767466952054787</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="D25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11245606200000002</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="2"/>
+        <v>0.83371085652054788</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="3">
+        <v>19</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>20</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>861</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <f t="shared" si="0"/>
         <v>0.86099999999999999</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
-        <v>7.3938375000000001E-2</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="2"/>
-        <v>0.79519316952054786</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14737392599999999</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.86862872052054785</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="3">
+        <v>20</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>21</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <v>659</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>0.65900000000000003</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
-        <v>5.6591625000000034E-2</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="2"/>
-        <v>0.77784641952054789</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="D27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11279839400000002</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>0.83405318852054788</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="3">
+        <v>21</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>22</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>1099</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <f t="shared" si="0"/>
         <v>1.099</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <f t="shared" si="1"/>
         <v>9.4376624999999992E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <f t="shared" si="2"/>
         <v>0.81563141952054785</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="3">
+        <v>22</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>23</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="8">
         <v>1834</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <f t="shared" si="0"/>
         <v>1.8340000000000001</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <f t="shared" si="1"/>
         <v>0.15749475000000002</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <f t="shared" si="2"/>
         <v>0.87874954452054788</v>
       </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="3">
+        <v>23</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+  </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug on xlsx formula. Tested script, working fine
</commit_message>
<xml_diff>
--- a/test_dia.xlsx
+++ b/test_dia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Belen/Dropbox/Programacion/Proyectos/Iberdrolux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C0B37C-C974-3749-8A46-A8627609EC72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B000DC3-24CB-AD46-A146-43DF04D41A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{282E9E91-F784-6B4B-BA20-4F197C46D5EC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Hora</t>
   </si>
@@ -50,12 +50,6 @@
     <t>TEST PARA EL DÍA:</t>
   </si>
   <si>
-    <t>Coste sin incluir potencia (€/h)</t>
-  </si>
-  <si>
-    <t>Coste incluyendo la potencia (€/h)</t>
-  </si>
-  <si>
     <t>Número días año:</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
     <t>Precio por kW/año de potencia (€):</t>
   </si>
   <si>
-    <t>COSTE TOTAL (€):</t>
-  </si>
-  <si>
     <t>Marque X si la hora está bonificada:</t>
   </si>
   <si>
@@ -84,6 +75,12 @@
   </si>
   <si>
     <t xml:space="preserve">CONSUMO TOTAL (kW): </t>
+  </si>
+  <si>
+    <t>Coste sin incluir la potencia (€/h)</t>
+  </si>
+  <si>
+    <t>COSTE TOTAL INCLUYENDO POTENCIA (€):</t>
   </si>
 </sst>
 </file>
@@ -319,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,7 +369,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,12 +685,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697522F4-44C9-8C4D-B60F-C35EB184269D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="167" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="167" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
@@ -712,14 +710,14 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="6">
         <v>365</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1">
         <v>0.17116600000000001</v>
@@ -728,11 +726,11 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" s="9">
-        <f>SUM(E6:E29)</f>
-        <v>18.86972923749315</v>
+        <f>SUM(D6:D29)+F2*F3/F1</f>
+        <v>2.2808689635205477</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
@@ -743,7 +741,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I2" s="6">
         <v>8.5875000000000007E-2</v>
@@ -751,8 +749,8 @@
     </row>
     <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="18" t="s">
-        <v>16</v>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <f>SUM(C6:C29)</f>
@@ -760,7 +758,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" s="8">
         <v>57.23</v>
@@ -791,15 +789,11 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>14</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I5" s="5"/>
     </row>
@@ -815,20 +809,15 @@
         <v>0.60199999999999998</v>
       </c>
       <c r="D6" s="2">
-        <f>E6-($F$2*$F$3/$F$1)</f>
-        <v>5.1696749999999958E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <f>IF(I6="X", C6*$I$2,C6*$I$1)+($F$2*$F$3/$F$1)</f>
-        <v>0.77295154452054782</v>
-      </c>
-      <c r="F6" s="1"/>
+        <f>IF(I6="X", C6*$I$2,C6*$I$1)</f>
+        <v>5.169675E-2</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3">
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -843,20 +832,15 @@
         <v>0.54800000000000004</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D29" si="1">E7-($F$2*$F$3/$F$1)</f>
-        <v>4.7059500000000032E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" ref="E7:E29" si="2">IF(I7="X", C7*$I$2,C7*$I$1)+($F$2*$F$3/$F$1)</f>
-        <v>0.76831429452054789</v>
-      </c>
-      <c r="F7" s="1"/>
+        <f>IF(I7="X", C7*$I$2,C7*$I$1)</f>
+        <v>4.7059500000000004E-2</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -871,20 +855,15 @@
         <v>0.94199999999999995</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
-        <v>8.0894250000000056E-2</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="2"/>
-        <v>0.80214904452054792</v>
-      </c>
-      <c r="F8" s="1"/>
+        <f>IF(I8="X", C8*$I$2,C8*$I$1)</f>
+        <v>8.0894250000000001E-2</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="3">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -899,20 +878,15 @@
         <v>0.64900000000000002</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
-        <v>5.5732875000000015E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="2"/>
-        <v>0.77698766952054787</v>
-      </c>
-      <c r="F9" s="1"/>
+        <f>IF(I9="X", C9*$I$2,C9*$I$1)</f>
+        <v>5.5732875000000008E-2</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3">
         <v>3</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -927,20 +901,15 @@
         <v>0.23300000000000001</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
-        <v>2.0008875000000037E-2</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="2"/>
-        <v>0.7412636695205479</v>
-      </c>
-      <c r="F10" s="1"/>
+        <f>IF(I10="X", C10*$I$2,C10*$I$1)</f>
+        <v>2.0008875000000002E-2</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3">
         <v>4</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -955,20 +924,15 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
-        <v>8.7592499999999962E-3</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.73001404452054786</v>
-      </c>
-      <c r="F11" s="1"/>
+        <f>IF(I11="X", C11*$I$2,C11*$I$1)</f>
+        <v>8.7592499999999997E-3</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3">
         <v>5</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -983,20 +947,15 @@
         <v>0.124</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.064849999999995E-2</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="2"/>
-        <v>0.73190329452054781</v>
-      </c>
-      <c r="F12" s="1"/>
+        <f>IF(I12="X", C12*$I$2,C12*$I$1)</f>
+        <v>1.06485E-2</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3">
         <v>6</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1011,20 +970,15 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>7.2993749999999968E-3</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="2"/>
-        <v>0.72855416952054786</v>
-      </c>
-      <c r="F13" s="1"/>
+        <f>IF(I13="X", C13*$I$2,C13*$I$1)</f>
+        <v>7.2993750000000012E-3</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3">
         <v>7</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1039,20 +993,15 @@
         <v>0.155</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
-        <v>1.331062500000002E-2</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.73456541952054788</v>
-      </c>
-      <c r="F14" s="1"/>
+        <f>IF(I14="X", C14*$I$2,C14*$I$1)</f>
+        <v>1.3310625000000001E-2</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3">
         <v>8</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1067,20 +1016,15 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
-        <v>2.4646124999999963E-2</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="2"/>
-        <v>0.74590091952054782</v>
-      </c>
-      <c r="F15" s="1"/>
+        <f>IF(I15="X", C15*$I$2,C15*$I$1)</f>
+        <v>2.4646125000000001E-2</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="3">
         <v>9</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1095,20 +1039,15 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
-        <v>2.0953499999999958E-2</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.74220829452054782</v>
-      </c>
-      <c r="F16" s="1"/>
+        <f>IF(I16="X", C16*$I$2,C16*$I$1)</f>
+        <v>2.09535E-2</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="3">
         <v>10</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1123,20 +1062,15 @@
         <v>0.28299999999999997</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
-        <v>2.4302625000000022E-2</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="2"/>
-        <v>0.74555741952054788</v>
-      </c>
-      <c r="F17" s="1"/>
+        <f>IF(I17="X", C17*$I$2,C17*$I$1)</f>
+        <v>2.4302625000000001E-2</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="3">
         <v>11</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1151,20 +1085,15 @@
         <v>0.65400000000000003</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
-        <v>5.6162249999999969E-2</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="2"/>
-        <v>0.77741704452054783</v>
-      </c>
-      <c r="F18" s="1"/>
+        <f>IF(I18="X", C18*$I$2,C18*$I$1)</f>
+        <v>5.6162250000000004E-2</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="3">
         <v>12</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1179,20 +1108,15 @@
         <v>0.48599999999999999</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
+        <f>IF(I19="X", C19*$I$2,C19*$I$1)</f>
         <v>4.1735250000000002E-2</v>
       </c>
-      <c r="E19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.76299004452054786</v>
-      </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="3">
         <v>13</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1207,14 +1131,9 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.13265364999999996</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.85390844452054782</v>
-      </c>
-      <c r="F20" s="1"/>
+        <f>IF(I20="X", C20*$I$2,C20*$I$1)</f>
+        <v>0.13265365000000001</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="3">
         <v>14</v>
@@ -1233,14 +1152,9 @@
         <v>0.69899999999999995</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11964503400000004</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.8408998285205479</v>
-      </c>
-      <c r="F21" s="1"/>
+        <f>IF(I21="X", C21*$I$2,C21*$I$1)</f>
+        <v>0.119645034</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="3">
         <v>15</v>
@@ -1259,14 +1173,9 @@
         <v>0.377</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="1"/>
-        <v>6.452958200000003E-2</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="2"/>
-        <v>0.78578437652054789</v>
-      </c>
-      <c r="F22" s="1"/>
+        <f>IF(I22="X", C22*$I$2,C22*$I$1)</f>
+        <v>6.4529582000000002E-2</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="3">
         <v>16</v>
@@ -1285,14 +1194,9 @@
         <v>0.314</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="1"/>
+        <f>IF(I23="X", C23*$I$2,C23*$I$1)</f>
         <v>5.3746124000000006E-2</v>
       </c>
-      <c r="E23" s="2">
-        <f t="shared" si="2"/>
-        <v>0.77500091852054787</v>
-      </c>
-      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="3">
         <v>17</v>
@@ -1311,14 +1215,9 @@
         <v>0.59199999999999997</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="1"/>
+        <f>IF(I24="X", C24*$I$2,C24*$I$1)</f>
         <v>0.101330272</v>
       </c>
-      <c r="E24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.82258506652054786</v>
-      </c>
-      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="3">
         <v>18</v>
@@ -1337,14 +1236,9 @@
         <v>0.65700000000000003</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11245606200000002</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="2"/>
-        <v>0.83371085652054788</v>
-      </c>
-      <c r="F25" s="1"/>
+        <f>IF(I25="X", C25*$I$2,C25*$I$1)</f>
+        <v>0.11245606200000001</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="3">
         <v>19</v>
@@ -1363,14 +1257,9 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14737392599999999</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="2"/>
-        <v>0.86862872052054785</v>
-      </c>
-      <c r="F26" s="1"/>
+        <f>IF(I26="X", C26*$I$2,C26*$I$1)</f>
+        <v>0.14737392600000002</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="3">
         <v>20</v>
@@ -1389,14 +1278,9 @@
         <v>0.65900000000000003</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11279839400000002</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="2"/>
-        <v>0.83405318852054788</v>
-      </c>
-      <c r="F27" s="1"/>
+        <f>IF(I27="X", C27*$I$2,C27*$I$1)</f>
+        <v>0.11279839400000001</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="3">
         <v>21</v>
@@ -1415,20 +1299,15 @@
         <v>1.099</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="1"/>
-        <v>9.4376624999999992E-2</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.81563141952054785</v>
-      </c>
-      <c r="F28" s="1"/>
+        <f>IF(I28="X", C28*$I$2,C28*$I$1)</f>
+        <v>9.4376625000000006E-2</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="3">
         <v>22</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1443,26 +1322,21 @@
         <v>1.8340000000000001</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="1"/>
+        <f>IF(I29="X", C29*$I$2,C29*$I$1)</f>
         <v>0.15749475000000002</v>
       </c>
-      <c r="E29" s="2">
-        <f t="shared" si="2"/>
-        <v>0.87874954452054788</v>
-      </c>
-      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="3">
         <v>23</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1470,7 +1344,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>

</xml_diff>

<commit_message>
Added printing at end, option to show details per day, fixed bug with decimal positions and testing for two days made
</commit_message>
<xml_diff>
--- a/test_dia.xlsx
+++ b/test_dia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Belen/Dropbox/Programacion/Proyectos/Iberdrolux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B000DC3-24CB-AD46-A146-43DF04D41A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE537F26-CD67-3F4F-8F88-36ABDA50B1CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{282E9E91-F784-6B4B-BA20-4F197C46D5EC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Hora</t>
   </si>
@@ -686,7 +686,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="C2" s="9">
         <f>SUM(D6:D29)+F2*F3/F1</f>
-        <v>2.2808689635205477</v>
+        <v>2.3223203895205478</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
@@ -1109,15 +1109,13 @@
       </c>
       <c r="D19" s="2">
         <f>IF(I19="X", C19*$I$2,C19*$I$1)</f>
-        <v>4.1735250000000002E-2</v>
+        <v>8.3186676000000001E-2</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="3">
         <v>13</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">

</xml_diff>